<commit_message>
Used Dataprovider only for TC_001. Updated.
</commit_message>
<xml_diff>
--- a/data/TC_001.xlsx
+++ b/data/TC_001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SYED SAMEER\eclipse-workspace\SalesAndInventoryTestNg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ADFA9A-DD7E-49C2-AC93-27346E409271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3112846E-EB82-486F-850F-6C543CB2D638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" xr2:uid="{8AC0E695-66C1-44AF-8598-247487E76A3C}"/>
   </bookViews>
@@ -49,22 +49,22 @@
     <t>8</t>
   </si>
   <si>
-    <t>Bangaloreoiu</t>
-  </si>
-  <si>
-    <t>Bangaloreqwe</t>
-  </si>
-  <si>
-    <t>Lifevb</t>
-  </si>
-  <si>
-    <t>Lifeyalk</t>
-  </si>
-  <si>
-    <t>9341224577</t>
-  </si>
-  <si>
-    <t>9764459999</t>
+    <t>Bangaloreeez</t>
+  </si>
+  <si>
+    <t>Bangaloreyyq</t>
+  </si>
+  <si>
+    <t>Lifeuuv</t>
+  </si>
+  <si>
+    <t>Lifeiima</t>
+  </si>
+  <si>
+    <t>9764454332</t>
+  </si>
+  <si>
+    <t>9341262932</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -476,7 +476,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>

</xml_diff>